<commit_message>
parabank test cases unfinished
</commit_message>
<xml_diff>
--- a/com.parabank/src/test/resources/test_data_parabank.xlsx
+++ b/com.parabank/src/test/resources/test_data_parabank.xlsx
@@ -8,13 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.parabank/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3129F89-9CFE-B34D-8A14-54E7678D0600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DF1161-BC8B-014B-A495-146718CA6E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="1" xr2:uid="{978947DF-1877-5E4D-ADCB-8EE592E5734F}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" firstSheet="1" activeTab="9" xr2:uid="{978947DF-1877-5E4D-ADCB-8EE592E5734F}"/>
   </bookViews>
   <sheets>
     <sheet name="AccountRegisteredSuccessfully" sheetId="1" r:id="rId1"/>
-    <sheet name="AccountOptions" sheetId="2" r:id="rId2"/>
+    <sheet name="CheckingAccount" sheetId="2" r:id="rId2"/>
+    <sheet name="SavingsAccount" sheetId="3" r:id="rId3"/>
+    <sheet name="AccountBalance" sheetId="4" r:id="rId4"/>
+    <sheet name="AccountType" sheetId="5" r:id="rId5"/>
+    <sheet name="TransferFunds" sheetId="6" r:id="rId6"/>
+    <sheet name="BillPayment" sheetId="7" r:id="rId7"/>
+    <sheet name="TransactionDate" sheetId="8" r:id="rId8"/>
+    <sheet name="UpdateProfile" sheetId="9" r:id="rId9"/>
+    <sheet name="ApplyForLoan" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Your account was created successfully. You are now logged in.</t>
   </si>
@@ -46,13 +54,67 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Congratulations, your account is now open.</t>
+  </si>
+  <si>
+    <t>Balance*</t>
+  </si>
+  <si>
+    <t>Account Type:</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>Transfer Complete!</t>
+  </si>
+  <si>
+    <t>Bill Payment Complete</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>Transaction Results</t>
+  </si>
+  <si>
+    <t>11-17-2022</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>1234 56th Ave</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>Profile Updated</t>
+  </si>
+  <si>
+    <t>Congratulations, your loan has been approved.</t>
+  </si>
+  <si>
+    <t>50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,6 +127,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,10 +154,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,7 +477,7 @@
   <dimension ref="A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -426,27 +495,265 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177B0C8E-7126-BE46-B2FA-4C07CE74BB68}">
+  <dimension ref="A2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="40" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F8F9F9B-B6E6-284F-BC04-8173F50F7F88}">
-  <dimension ref="A2:A3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="10.83203125" style="2"/>
-  </cols>
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="58" style="2" customWidth="1"/>
+    <col min="3" max="3" width="51.33203125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9614D37-A897-2741-979C-B6F3D59B3D53}">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="50.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E412EFDD-07BC-A449-9C90-3446ECC93A2C}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE4C6710-E6F5-3D4E-A560-4E7A70892F49}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6A1439-9D26-6F47-A42B-A57A3EC0969C}">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445276BB-1D57-4648-9583-9DAEBCF7C925}">
+  <dimension ref="A2:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258B98D1-A682-A943-BA78-B050B3F14798}">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="18" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A5505F-B759-D94D-BEF7-8FF27F3A5923}">
+  <dimension ref="A2:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="14.5" style="2" customWidth="1"/>
+    <col min="4" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2">
+        <v>12345</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1111111111</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>